<commit_message>
Corrected priority queue and added Raport.docx + Classeur1.xlsx
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Windows7\stud.II\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="12585"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -45,8 +50,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,16 +101,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -129,18 +152,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>AVG</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Feuil1!$B$1:$D$1</c:f>
@@ -162,7 +189,7 @@
             <c:numRef>
               <c:f>Feuil1!$B$24:$D$24</c:f>
               <c:numCache>
-                <c:formatCode>Standardowy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>2.0826919545454547</c:v>
@@ -177,32 +204,49 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="82752256"/>
-        <c:axId val="82753792"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="621637008"/>
+        <c:axId val="621302480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82752256"/>
+        <c:axId val="621637008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82753792"/>
+        <c:crossAx val="621302480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82753792"/>
+        <c:axId val="621302480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="Standardowy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82752256"/>
+        <c:crossAx val="621637008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -210,8 +254,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -223,7 +270,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -257,7 +314,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Grafik reprezentujący średni czas wysłania pakietu w zależności od algorytmu kolejkowania dla rozkładu On- Off</a:t>
+              <a:t>Porównanie wszytkich rozkładów generowania ruchu oraz alogorymów kolejkowania</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
           </a:p>
@@ -286,23 +343,27 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>AVG</c:v>
+            <c:v>AVG ON-OFF</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Feuil1!$G$1:$H$1</c:f>
@@ -321,7 +382,7 @@
             <c:numRef>
               <c:f>Feuil1!$G$22:$H$22</c:f>
               <c:numCache>
-                <c:formatCode>Standardowy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>14.039641525000002</c:v>
@@ -333,32 +394,166 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="133744896"/>
-        <c:axId val="133746688"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>AVG Poisson</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Fifo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lifo</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Priority</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$24:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.0826919545454547</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7404646000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6868318636363631</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>AVG Wkładniczy</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$L$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Fifo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lifo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$L$24:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5.2363449450000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.371246197727273</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>AVG MMPP</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$Q$1:$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Fifo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lifo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$Q$24:$R$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.7742181363636365</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4724053636363637</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="622222176"/>
+        <c:axId val="723966816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133744896"/>
+        <c:axId val="622222176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133746688"/>
+        <c:crossAx val="723966816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133746688"/>
+        <c:axId val="723966816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="Standardowy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133744896"/>
+        <c:crossAx val="622222176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -366,12 +561,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -379,7 +577,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -447,18 +655,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>AVG</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Feuil1!$L$1:$M$1</c:f>
@@ -477,7 +689,7 @@
             <c:numRef>
               <c:f>Feuil1!$L$24:$M$24</c:f>
               <c:numCache>
-                <c:formatCode>Standardowy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>5.2363449450000008</c:v>
@@ -489,32 +701,49 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="134479232"/>
-        <c:axId val="133612288"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="621306960"/>
+        <c:axId val="621307520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134479232"/>
+        <c:axId val="621306960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133612288"/>
+        <c:crossAx val="621307520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133612288"/>
+        <c:axId val="621307520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="Standardowy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134479232"/>
+        <c:crossAx val="621306960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -522,8 +751,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -535,7 +767,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -603,18 +845,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>AVG</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Feuil1!$Q$1:$R$1</c:f>
@@ -633,7 +879,7 @@
             <c:numRef>
               <c:f>Feuil1!$Q$24:$R$24</c:f>
               <c:numCache>
-                <c:formatCode>Standardowy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1.7742181363636365</c:v>
@@ -645,32 +891,49 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="161408512"/>
-        <c:axId val="161410048"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="719092064"/>
+        <c:axId val="719092624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="161408512"/>
+        <c:axId val="719092064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161410048"/>
+        <c:crossAx val="719092624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161410048"/>
+        <c:axId val="719092624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="Standardowy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161408512"/>
+        <c:crossAx val="719092064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -678,8 +941,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -815,9 +1081,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -855,9 +1121,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -889,9 +1155,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -923,9 +1190,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1098,19 +1366,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>1.1972339999999999</v>
@@ -1196,7 +1464,7 @@
       </c>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>1.6379680000000001</v>
@@ -1232,7 +1500,7 @@
       </c>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>1.6479330000000001</v>
@@ -1268,7 +1536,7 @@
       </c>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>2.574592</v>
@@ -1304,7 +1572,7 @@
       </c>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>1.0979639999999999</v>
@@ -1340,7 +1608,7 @@
       </c>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2.9066900000000002</v>
@@ -1376,7 +1644,7 @@
       </c>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>1.7945679999999999</v>
@@ -1412,7 +1680,7 @@
       </c>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>3.1225640000000001</v>
@@ -1448,7 +1716,7 @@
       </c>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>1.745207</v>
@@ -1484,7 +1752,7 @@
       </c>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>1.6139060000000001</v>
@@ -1520,7 +1788,7 @@
       </c>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>1.075496</v>
@@ -1556,7 +1824,7 @@
       </c>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>2.6893940000000001</v>
@@ -1592,7 +1860,7 @@
       </c>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>1.1262179999999999</v>
@@ -1629,7 +1897,7 @@
       </c>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>1.8291409999999999</v>
@@ -1665,7 +1933,7 @@
       </c>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>1.5785229999999999</v>
@@ -1701,7 +1969,7 @@
       </c>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>2.086878</v>
@@ -1737,7 +2005,7 @@
       </c>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>1.2166760000000001</v>
@@ -1773,7 +2041,7 @@
       </c>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>1.925009</v>
@@ -1809,7 +2077,7 @@
       </c>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>5.2681950000000004</v>
@@ -1845,7 +2113,7 @@
       </c>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>1.368571</v>
@@ -1881,7 +2149,7 @@
       </c>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>1.350284</v>
@@ -1925,7 +2193,7 @@
       </c>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>4.9662119999999996</v>
@@ -1953,7 +2221,7 @@
       </c>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -2013,24 +2281,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Elements can be nodes (white) or generators (black)
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Windows7\stud.II\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -50,8 +45,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,7 +96,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -118,135 +113,58 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t>Grafik</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" baseline="0"/>
-              <a:t> reprezentujący średni czas wysłania pakietu w zależności od algorytmu kolejkowania dla rozkładu Poissona</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>AVG</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Feuil1!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Fifo</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Lifo</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Priority</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$24:$D$24</c:f>
+              <c:f>Feuil1!$B$24:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2.0826919545454547</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.7404646000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.6868318636363631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="621637008"/>
-        <c:axId val="621302480"/>
+        <c:axId val="77600256"/>
+        <c:axId val="77601792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="621637008"/>
+        <c:axId val="77600256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="621302480"/>
+        <c:crossAx val="77601792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="621302480"/>
+        <c:axId val="77601792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="621637008"/>
+        <c:crossAx val="77600256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -254,11 +172,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -270,100 +185,173 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Porównanie wszytkich rozkładów generowania ruchu oraz alogorymów kolejkowania</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$G$24:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>13.956542850000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.249641078947372</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="86074496"/>
+        <c:axId val="86076032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="86074496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86076032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86076032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86074496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$L$22:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4.4398860000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2363449450000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="82476032"/>
+        <c:axId val="84469248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="82476032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84469248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84469248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82476032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1431795896628764E-2"/>
+          <c:y val="0.30249868943913094"/>
+          <c:w val="0.69553822293736511"/>
+          <c:h val="0.60739589643637892"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
-            <c:v>AVG ON-OFF</c:v>
+            <c:v>MMPP</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Feuil1!$G$1:$H$1</c:f>
@@ -373,124 +361,7 @@
                   <c:v>Fifo</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Lifo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Feuil1!$G$22:$H$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>14.039641525000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.956542850000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>AVG Poisson</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Feuil1!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Fifo</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Lifo</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>Priority</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Feuil1!$B$24:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2.0826919545454547</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.7404646000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.6868318636363631</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>AVG Wkładniczy</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Feuil1!$L$1:$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Fifo</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Lifo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Feuil1!$L$24:$M$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>5.2363449450000008</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.371246197727273</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>AVG MMPP</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Feuil1!$Q$1:$R$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Fifo</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Lifo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -511,49 +382,140 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="622222176"/>
-        <c:axId val="723966816"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Wykladniczy</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Fifo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Priority</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$L$22:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4.4398860000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2363449450000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>On-Off</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Fifo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Priority</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$G$24:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>13.956542850000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.249641078947372</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Poisson</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Fifo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Priority</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$24:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.0826919545454547</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7404646000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="107112704"/>
+        <c:axId val="107123072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="622222176"/>
+        <c:axId val="107112704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="723966816"/>
+        <c:crossAx val="107123072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="723966816"/>
+        <c:axId val="107123072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="622222176"/>
+        <c:crossAx val="107112704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -561,391 +523,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Grafik reprezentujący średni czas wysłania pakietu w zależności od algorytmu kolejkowania dla rozkładu Wykładniczego</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>AVG</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Feuil1!$L$1:$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Fifo</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Lifo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Feuil1!$L$24:$M$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>5.2363449450000008</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.371246197727273</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="621306960"/>
-        <c:axId val="621307520"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="621306960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="621307520"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="621307520"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="621306960"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Grafik reprezentujący średni czas wysłania pakietu w zależności od algorytmu kolejkowania dla rozkładu MMPP</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>AVG</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Feuil1!$Q$1:$R$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Fifo</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Lifo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Feuil1!$Q$24:$R$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.7742181363636365</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.4724053636363637</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="719092064"/>
-        <c:axId val="719092624"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="719092064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="719092624"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="719092624"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="719092064"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -959,20 +538,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>217714</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvPr id="8" name="Chart 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -989,20 +568,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>576943</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:colOff>446315</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Graphique 4"/>
+        <xdr:cNvPr id="9" name="Chart 8"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1020,19 +599,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:colOff>43542</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>696685</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Graphique 5"/>
+        <xdr:cNvPr id="10" name="Chart 9"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1050,19 +629,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>370114</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>239485</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Graphique 6"/>
+        <xdr:cNvPr id="11" name="Chart 10"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1081,9 +660,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1121,9 +700,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1155,10 +734,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1190,10 +768,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1366,19 +943,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W9" sqref="W8:W9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1398,10 +975,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>5</v>
@@ -1410,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>4</v>
@@ -1419,7 +996,7 @@
         <v>6</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>2</v>
@@ -1428,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>1.1972339999999999</v>
@@ -1437,24 +1014,28 @@
         <v>1.0614710000000001</v>
       </c>
       <c r="D2" s="1">
-        <v>3.0219879999999999</v>
+        <v>1.0614710000000001</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1">
-        <v>10.04965</v>
+        <v>10.000181</v>
       </c>
       <c r="H2" s="1">
+        <v>10.054795</v>
+      </c>
+      <c r="I2" s="1">
         <v>10.000181</v>
       </c>
-      <c r="I2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1">
+        <v>3.3776540000000002</v>
+      </c>
+      <c r="M2" s="1">
         <v>4.0223449999999996</v>
       </c>
-      <c r="M2" s="1">
-        <v>3.3776540000000002</v>
-      </c>
-      <c r="N2" s="1"/>
+      <c r="N2" s="1">
+        <v>4.0223449999999996</v>
+      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1">
         <v>1.009026</v>
@@ -1464,7 +1045,7 @@
       </c>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>1.6379680000000001</v>
@@ -1473,24 +1054,28 @@
         <v>1.8804339999999999</v>
       </c>
       <c r="D3" s="1">
-        <v>3.4504419999999998</v>
+        <v>1.8804339999999999</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1">
-        <v>10.054795</v>
+        <v>10.000181</v>
       </c>
       <c r="H3" s="1">
+        <v>11.946542000000001</v>
+      </c>
+      <c r="I3" s="1">
         <v>10.000181</v>
       </c>
-      <c r="I3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1">
+        <v>3.6452800000000001</v>
+      </c>
+      <c r="M3" s="1">
         <v>4.3345640000000003</v>
       </c>
-      <c r="M3" s="1">
-        <v>3.6452800000000001</v>
-      </c>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1">
+        <v>4.3345640000000003</v>
+      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1">
         <v>1.028465</v>
@@ -1500,7 +1085,7 @@
       </c>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>1.6479330000000001</v>
@@ -1509,24 +1094,28 @@
         <v>2.240472</v>
       </c>
       <c r="D4" s="1">
-        <v>4.0759030000000003</v>
+        <v>2.240472</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1">
-        <v>11.946542000000001</v>
+        <v>10.000181</v>
       </c>
       <c r="H4" s="1">
+        <v>17.465446</v>
+      </c>
+      <c r="I4" s="1">
         <v>10.000181</v>
       </c>
-      <c r="I4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1">
+        <v>5.3654489999999999</v>
+      </c>
+      <c r="M4" s="1">
         <v>5.8641459999999999</v>
       </c>
-      <c r="M4" s="1">
-        <v>5.3654489999999999</v>
-      </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="1">
+        <v>5.8641459999999999</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1">
         <v>1.3345640000000001</v>
@@ -1536,7 +1125,7 @@
       </c>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>2.574592</v>
@@ -1545,24 +1134,28 @@
         <v>2.5156040000000002</v>
       </c>
       <c r="D5" s="1">
-        <v>5.5220510000000003</v>
+        <v>2.5156040000000002</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1">
-        <v>17.465446</v>
+        <v>10.000181</v>
       </c>
       <c r="H5" s="1">
+        <v>10.165445</v>
+      </c>
+      <c r="I5" s="1">
         <v>10.000181</v>
       </c>
-      <c r="I5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1">
+        <v>6.2146540000000003</v>
+      </c>
+      <c r="M5" s="1">
         <v>6.0468760000000001</v>
       </c>
-      <c r="M5" s="1">
-        <v>6.2146540000000003</v>
-      </c>
-      <c r="N5" s="1"/>
+      <c r="N5" s="1">
+        <v>6.0468760000000001</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1">
         <v>1.863375</v>
@@ -1572,7 +1165,7 @@
       </c>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>1.0979639999999999</v>
@@ -1581,24 +1174,28 @@
         <v>1.6512579999999999</v>
       </c>
       <c r="D6" s="1">
-        <v>3.3281459999999998</v>
+        <v>1.6512579999999999</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1">
-        <v>10.165445</v>
+        <v>11.900373</v>
       </c>
       <c r="H6" s="1">
+        <v>10.065445</v>
+      </c>
+      <c r="I6" s="1">
         <v>11.900373</v>
       </c>
-      <c r="I6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1">
+        <v>3.9144649999999999</v>
+      </c>
+      <c r="M6" s="1">
         <v>6.7541320000000002</v>
       </c>
-      <c r="M6" s="1">
-        <v>3.9144649999999999</v>
-      </c>
-      <c r="N6" s="1"/>
+      <c r="N6" s="1">
+        <v>6.7541320000000002</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1">
         <v>1.126544</v>
@@ -1608,7 +1205,7 @@
       </c>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>2.9066900000000002</v>
@@ -1617,24 +1214,28 @@
         <v>3.282518</v>
       </c>
       <c r="D7" s="1">
-        <v>4.3836120000000003</v>
+        <v>3.282518</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1">
-        <v>10.065445</v>
+        <v>10.008787</v>
       </c>
       <c r="H7" s="1">
+        <v>10.000654000000001</v>
+      </c>
+      <c r="I7" s="1">
         <v>10.008787</v>
       </c>
-      <c r="I7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1">
+        <v>4.1456540000000004</v>
+      </c>
+      <c r="M7" s="1">
         <v>5.5113539999999999</v>
       </c>
-      <c r="M7" s="1">
-        <v>4.1456540000000004</v>
-      </c>
-      <c r="N7" s="1"/>
+      <c r="N7" s="1">
+        <v>5.5113539999999999</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1">
         <v>1.064435</v>
@@ -1644,7 +1245,7 @@
       </c>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>1.7945679999999999</v>
@@ -1653,24 +1254,28 @@
         <v>1.0611812</v>
       </c>
       <c r="D8" s="1">
-        <v>3.4019159999999999</v>
+        <v>1.0611812</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1">
-        <v>10.000654000000001</v>
+        <v>10.008787</v>
       </c>
       <c r="H8" s="1">
+        <v>9.9999415999999997</v>
+      </c>
+      <c r="I8" s="1">
         <v>10.008787</v>
       </c>
-      <c r="I8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1">
+        <v>2.9410639999999999</v>
+      </c>
+      <c r="M8" s="1">
         <v>5.1654460000000002</v>
       </c>
-      <c r="M8" s="1">
-        <v>2.9410639999999999</v>
-      </c>
-      <c r="N8" s="1"/>
+      <c r="N8" s="1">
+        <v>5.1654460000000002</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1">
         <v>2.161108</v>
@@ -1680,7 +1285,7 @@
       </c>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>3.1225640000000001</v>
@@ -1689,24 +1294,28 @@
         <v>1.590284</v>
       </c>
       <c r="D9" s="1">
-        <v>6.9651639999999997</v>
+        <v>1.590284</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1">
-        <v>9.9999415999999997</v>
+        <v>10.008787</v>
       </c>
       <c r="H9" s="1">
+        <v>9.9999859000000004</v>
+      </c>
+      <c r="I9" s="1">
         <v>10.008787</v>
       </c>
-      <c r="I9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1">
+        <v>5.314654</v>
+      </c>
+      <c r="M9" s="1">
         <v>4.8234450000000004</v>
       </c>
-      <c r="M9" s="1">
-        <v>5.314654</v>
-      </c>
-      <c r="N9" s="1"/>
+      <c r="N9" s="1">
+        <v>4.8234450000000004</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1">
         <v>1.4286449999999999</v>
@@ -1716,7 +1325,7 @@
       </c>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>1.745207</v>
@@ -1725,24 +1334,28 @@
         <v>1.341135</v>
       </c>
       <c r="D10" s="1">
-        <v>5.3254159999999997</v>
+        <v>1.341135</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
-        <v>9.9999859000000004</v>
+        <v>11.076088</v>
       </c>
       <c r="H10" s="1">
+        <v>30.827165999999998</v>
+      </c>
+      <c r="I10" s="1">
         <v>11.076088</v>
       </c>
-      <c r="I10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1">
+        <v>1.214564</v>
+      </c>
+      <c r="M10" s="1">
         <v>4.7765449999999996</v>
       </c>
-      <c r="M10" s="1">
-        <v>1.214564</v>
-      </c>
-      <c r="N10" s="1"/>
+      <c r="N10" s="1">
+        <v>4.7765449999999996</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1">
         <v>1.110044</v>
@@ -1752,7 +1365,7 @@
       </c>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>1.6139060000000001</v>
@@ -1761,24 +1374,28 @@
         <v>1.881645</v>
       </c>
       <c r="D11" s="1">
-        <v>6.6545459999999999</v>
+        <v>1.881645</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1">
-        <v>30.827165999999998</v>
+        <v>10.162032999999999</v>
       </c>
       <c r="H11" s="1">
+        <v>10.000031</v>
+      </c>
+      <c r="I11" s="1">
         <v>10.162032999999999</v>
       </c>
-      <c r="I11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1">
+        <v>4.5649839999999999</v>
+      </c>
+      <c r="M11" s="1">
         <v>6.7954309999999998</v>
       </c>
-      <c r="M11" s="1">
-        <v>4.5649839999999999</v>
-      </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="1">
+        <v>6.7954309999999998</v>
+      </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1">
         <v>2.113308</v>
@@ -1788,7 +1405,7 @@
       </c>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>1.075496</v>
@@ -1797,24 +1414,28 @@
         <v>5.2465840000000004</v>
       </c>
       <c r="D12" s="1">
-        <v>8.1465139999999998</v>
+        <v>5.2465840000000004</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1">
+        <v>10.162032999999999</v>
+      </c>
+      <c r="H12" s="1">
         <v>10.000031</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>10.162032999999999</v>
       </c>
-      <c r="I12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1">
+        <v>4.4865409999999999</v>
+      </c>
+      <c r="M12" s="1">
         <v>3.4564214</v>
       </c>
-      <c r="M12" s="1">
-        <v>4.4865409999999999</v>
-      </c>
-      <c r="N12" s="1"/>
+      <c r="N12" s="1">
+        <v>3.4564214</v>
+      </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1">
         <v>1.184652</v>
@@ -1824,7 +1445,7 @@
       </c>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>2.6893940000000001</v>
@@ -1833,24 +1454,28 @@
         <v>1.962145</v>
       </c>
       <c r="D13" s="1">
-        <v>3.2654540000000001</v>
+        <v>1.962145</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1">
-        <v>10.000031</v>
+        <v>21.094698000000001</v>
       </c>
       <c r="H13" s="1">
+        <v>9.9999959999999994</v>
+      </c>
+      <c r="I13" s="1">
         <v>21.094698000000001</v>
       </c>
-      <c r="I13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1">
+        <v>6.066465</v>
+      </c>
+      <c r="M13" s="1">
         <v>6.1259870000000003</v>
       </c>
-      <c r="M13" s="1">
-        <v>6.066465</v>
-      </c>
-      <c r="N13" s="1"/>
+      <c r="N13" s="1">
+        <v>6.1259870000000003</v>
+      </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1">
         <v>1.846522</v>
@@ -1860,7 +1485,7 @@
       </c>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>1.1262179999999999</v>
@@ -1869,25 +1494,28 @@
         <v>5.4516450000000001</v>
       </c>
       <c r="D14" s="1">
-        <v>4.1654650000000002</v>
+        <v>5.4516450000000001</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1">
-        <v>9.9999959999999994</v>
+        <v>9.9999730000000007</v>
       </c>
       <c r="H14" s="1">
+        <v>9.9999660000000006</v>
+      </c>
+      <c r="I14" s="1">
         <v>9.9999730000000007</v>
       </c>
-      <c r="I14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1">
+        <v>3.4554879999999999</v>
+      </c>
+      <c r="M14" s="1">
         <v>4.5249839999999999</v>
       </c>
-      <c r="M14" s="1">
-        <f>AVERAGE(B2:B23)</f>
-        <v>2.0826919545454547</v>
-      </c>
-      <c r="N14" s="1"/>
+      <c r="N14" s="1">
+        <v>4.5249839999999999</v>
+      </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1">
         <v>1.0974649999999999</v>
@@ -1897,7 +1525,7 @@
       </c>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>1.8291409999999999</v>
@@ -1906,24 +1534,28 @@
         <v>1.596452</v>
       </c>
       <c r="D15" s="1">
-        <v>4.2654459999999998</v>
+        <v>1.596452</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1">
-        <v>9.9999660000000006</v>
+        <v>22.333279000000001</v>
       </c>
       <c r="H15" s="1">
+        <v>60.217674000000002</v>
+      </c>
+      <c r="I15" s="1">
         <v>22.333279000000001</v>
       </c>
-      <c r="I15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1">
+        <v>2.7984619999999998</v>
+      </c>
+      <c r="M15" s="1">
         <v>5.1846546</v>
       </c>
-      <c r="M15" s="1">
-        <v>2.7984619999999998</v>
-      </c>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1">
+        <v>5.1846546</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1">
         <v>6.3455459999999997</v>
@@ -1933,7 +1565,7 @@
       </c>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>1.5785229999999999</v>
@@ -1942,24 +1574,28 @@
         <v>6.2100809999999997</v>
       </c>
       <c r="D16" s="1">
-        <v>7.1164639999999997</v>
+        <v>6.2100809999999997</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1">
-        <v>60.217674000000002</v>
+        <v>9.999962</v>
       </c>
       <c r="H16" s="1">
+        <v>9.9999959999999994</v>
+      </c>
+      <c r="I16" s="1">
         <v>9.999962</v>
       </c>
-      <c r="I16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1">
+        <v>5.7445639999999996</v>
+      </c>
+      <c r="M16" s="1">
         <v>6.3054654000000001</v>
       </c>
-      <c r="M16" s="1">
-        <v>5.7445639999999996</v>
-      </c>
-      <c r="N16" s="1"/>
+      <c r="N16" s="1">
+        <v>6.3054654000000001</v>
+      </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1">
         <v>1.0521210000000001</v>
@@ -1969,7 +1605,7 @@
       </c>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>2.086878</v>
@@ -1978,24 +1614,28 @@
         <v>1.0280130000000001</v>
       </c>
       <c r="D17" s="1">
-        <v>9.1654409999999995</v>
+        <v>1.0280130000000001</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1">
-        <v>9.9999959999999994</v>
+        <v>9.999962</v>
       </c>
       <c r="H17" s="1">
+        <v>9.9999660000000006</v>
+      </c>
+      <c r="I17" s="1">
         <v>9.999962</v>
       </c>
-      <c r="I17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1">
+        <v>4.7854619999999999</v>
+      </c>
+      <c r="M17" s="1">
         <v>5.8465449999999999</v>
       </c>
-      <c r="M17" s="1">
-        <v>4.7854619999999999</v>
-      </c>
-      <c r="N17" s="1"/>
+      <c r="N17" s="1">
+        <v>5.8465449999999999</v>
+      </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1">
         <v>2.44584</v>
@@ -2005,7 +1645,7 @@
       </c>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>1.2166760000000001</v>
@@ -2014,24 +1654,28 @@
         <v>3.1337640000000002</v>
       </c>
       <c r="D18" s="1">
-        <v>4.4154650000000002</v>
+        <v>3.1337640000000002</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1">
-        <v>9.9999660000000006</v>
+        <v>9.999962</v>
       </c>
       <c r="H18" s="1">
+        <v>10.000031</v>
+      </c>
+      <c r="I18" s="1">
         <v>9.999962</v>
       </c>
-      <c r="I18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1">
+        <v>4.245654</v>
+      </c>
+      <c r="M18" s="1">
         <v>5.0546544999999998</v>
       </c>
-      <c r="M18" s="1">
-        <v>4.245654</v>
-      </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1">
+        <v>5.0546544999999998</v>
+      </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1">
         <v>1.034565</v>
@@ -2041,7 +1685,7 @@
       </c>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>1.925009</v>
@@ -2050,24 +1694,28 @@
         <v>3.2663989999999998</v>
       </c>
       <c r="D19" s="1">
-        <v>3.146954</v>
+        <v>3.2663989999999998</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1">
+        <v>10.00034</v>
+      </c>
+      <c r="H19" s="1">
         <v>10.000031</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>10.00034</v>
       </c>
-      <c r="I19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1">
+        <v>6.104654</v>
+      </c>
+      <c r="M19" s="1">
         <v>4.4526539999999999</v>
       </c>
-      <c r="M19" s="1">
-        <v>6.104654</v>
-      </c>
-      <c r="N19" s="1"/>
+      <c r="N19" s="1">
+        <v>4.4526539999999999</v>
+      </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1">
         <v>1.1545650000000001</v>
@@ -2077,7 +1725,7 @@
       </c>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>5.2681950000000004</v>
@@ -2086,24 +1734,28 @@
         <v>2.294565</v>
       </c>
       <c r="D20" s="1">
-        <v>3.1654680000000002</v>
+        <v>2.294565</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1">
-        <v>10.000031</v>
+        <v>10.000054</v>
       </c>
       <c r="H20" s="1">
+        <v>10.000038</v>
+      </c>
+      <c r="I20" s="1">
         <v>10.000054</v>
       </c>
-      <c r="I20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1">
+        <v>5.8465480000000003</v>
+      </c>
+      <c r="M20" s="1">
         <v>6.6246840000000002</v>
       </c>
-      <c r="M20" s="1">
-        <v>5.8465480000000003</v>
-      </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1">
+        <v>6.6246840000000002</v>
+      </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1">
         <v>4.2694580000000002</v>
@@ -2113,7 +1765,7 @@
       </c>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>1.368571</v>
@@ -2122,24 +1774,29 @@
         <v>1.7964519999999999</v>
       </c>
       <c r="D21" s="1">
-        <v>3.2465440000000001</v>
+        <v>1.7964519999999999</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1">
-        <v>10.000038</v>
+        <v>62.375014999999998</v>
       </c>
       <c r="H21" s="1">
+        <f>AVERAGE(H1:H20)</f>
+        <v>14.249641078947372</v>
+      </c>
+      <c r="I21" s="1">
         <v>62.375014999999998</v>
       </c>
-      <c r="I21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1">
+        <v>4.5654599999999999</v>
+      </c>
+      <c r="M21" s="1">
         <v>3.056565</v>
       </c>
-      <c r="M21" s="1">
-        <v>4.5654599999999999</v>
-      </c>
-      <c r="N21" s="1"/>
+      <c r="N21" s="1">
+        <v>3.056565</v>
+      </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1">
         <v>2.1762419999999998</v>
@@ -2149,7 +1806,7 @@
       </c>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>1.350284</v>
@@ -2158,32 +1815,38 @@
         <v>3.3054649999999999</v>
       </c>
       <c r="D22" s="1">
-        <v>3.4164560000000002</v>
+        <v>3.3054649999999999</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G22" s="1">
         <f>AVERAGE(G2:G21)</f>
-        <v>14.039641525000002</v>
+        <v>13.956542850000002</v>
       </c>
       <c r="H22" s="1">
         <f>AVERAGE(H2:H21)</f>
+        <v>14.249641078947372</v>
+      </c>
+      <c r="I22" s="1">
+        <f>AVERAGE(I2:I21)</f>
         <v>13.956542850000002</v>
       </c>
-      <c r="I22" s="1"/>
       <c r="K22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L22" s="1">
         <f>AVERAGE(L2:L21)</f>
-        <v>5.2363449450000008</v>
+        <v>4.4398860000000004</v>
       </c>
       <c r="M22" s="1">
         <f>AVERAGE(M2:M21)</f>
-        <v>4.371246197727273</v>
-      </c>
-      <c r="N22" s="1"/>
+        <v>5.2363449450000008</v>
+      </c>
+      <c r="N22" s="1">
+        <f>AVERAGE(N2:N21)</f>
+        <v>5.2363449450000008</v>
+      </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1">
         <v>1.011754</v>
@@ -2193,7 +1856,7 @@
       </c>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>4.9662119999999996</v>
@@ -2202,7 +1865,7 @@
         <v>6.4926539999999999</v>
       </c>
       <c r="D23" s="1">
-        <v>3.465446</v>
+        <v>6.4926539999999999</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -2221,7 +1884,7 @@
       </c>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -2235,31 +1898,31 @@
       </c>
       <c r="D24" s="1">
         <f>AVERAGE(D2:D23)</f>
-        <v>4.6868318636363631</v>
+        <v>2.7404646000000001</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G24" s="1">
         <f>AVERAGE(G2:G23)</f>
-        <v>14.039641525</v>
+        <v>13.956542850000002</v>
       </c>
       <c r="H24" s="1">
         <f>AVERAGE(H2:H21)</f>
+        <v>14.249641078947372</v>
+      </c>
+      <c r="I24" s="1">
+        <f>AVERAGE(I2:I21)</f>
         <v>13.956542850000002</v>
       </c>
-      <c r="I24" s="1"/>
       <c r="K24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L24" s="1">
         <f>AVERAGE(L2:L23)</f>
-        <v>5.2363449450000008</v>
-      </c>
-      <c r="M24" s="1">
-        <f>AVERAGE(M2:M21)</f>
-        <v>4.371246197727273</v>
-      </c>
+        <v>4.4398860000000004</v>
+      </c>
+      <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="P24" s="1" t="s">
         <v>7</v>
@@ -2273,6 +1936,9 @@
         <v>1.4724053636363637</v>
       </c>
       <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="M25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2281,24 +1947,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>